<commit_message>
Update drug database, SUMMARY.md and changelog.md
</commit_message>
<xml_diff>
--- a/exclude.xlsx
+++ b/exclude.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$A$128</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>EALC752</t>
   </si>
@@ -350,13 +353,67 @@
   <si>
     <t>藥品代碼</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OCODIBAD</t>
+  </si>
+  <si>
+    <t>INS250</t>
+  </si>
+  <si>
+    <t>INS2</t>
+  </si>
+  <si>
+    <t>INS45/20</t>
+  </si>
+  <si>
+    <t>INSO100</t>
+  </si>
+  <si>
+    <t>INS5</t>
+  </si>
+  <si>
+    <t>INSO5</t>
+  </si>
+  <si>
+    <t>INS1</t>
+  </si>
+  <si>
+    <t>INS45</t>
+  </si>
+  <si>
+    <t>IGS5</t>
+  </si>
+  <si>
+    <t>IWAT500</t>
+  </si>
+  <si>
+    <t>IWAT</t>
+  </si>
+  <si>
+    <t>IGS33</t>
+  </si>
+  <si>
+    <t>IGS25</t>
+  </si>
+  <si>
+    <t>ESWI</t>
+  </si>
+  <si>
+    <t>ENS3</t>
+  </si>
+  <si>
+    <t>ENS2</t>
+  </si>
+  <si>
+    <t>IRL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,19 +436,28 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -411,10 +477,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -422,7 +486,18 @@
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="一般 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -698,566 +773,663 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A110"/>
+  <dimension ref="A1:A128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>